<commit_message>
Graphs and graph generation
and presentation and report backup
</commit_message>
<xml_diff>
--- a/graphs/Summary graphs.xlsx
+++ b/graphs/Summary graphs.xlsx
@@ -2,44 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/933150a7dfc8eecd/Documents/University of Missouri/Fall 2015/Unsupervised Learning/Unsupervised-Learning-Final/graphs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\OneDrive\Documents\University of Missouri\Fall 2015\Unsupervised Learning\Unsupervised-Learning-Final\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="1"/>
+    <workbookView xWindow="2415" yWindow="240" windowWidth="22380" windowHeight="14580"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart2" sheetId="5" r:id="rId1"/>
+    <sheet name="Unnormalized" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId3"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="23">
   <si>
     <t>Dataset</t>
   </si>
   <si>
-    <t>Hierarchical</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Cophenet</t>
+    <t>Clustering</t>
   </si>
   <si>
     <t>Method</t>
@@ -48,34 +45,22 @@
     <t>Measure</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>Unnormalized</t>
   </si>
   <si>
-    <t>K-Mediods</t>
+    <t>Normalized</t>
   </si>
   <si>
-    <t>Fuzzy K-med</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Clustering</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>Sum of Value</t>
+    <t>% improvement</t>
   </si>
   <si>
     <t>39 MFCCs</t>
   </si>
   <si>
-    <t>13 MFCCs</t>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Hierarchical</t>
   </si>
   <si>
     <t>NMI</t>
@@ -83,12 +68,48 @@
   <si>
     <t>Word</t>
   </si>
+  <si>
+    <t>Naïve accuracy</t>
+  </si>
+  <si>
+    <t>Cophenet</t>
+  </si>
+  <si>
+    <t>Sum of Normalized</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>K-Mediods</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Fuzzy C-Med</t>
+  </si>
+  <si>
+    <t>too low!</t>
+  </si>
+  <si>
+    <t>13 MFCCs</t>
+  </si>
+  <si>
+    <t>Fuzzy C-Med2</t>
+  </si>
+  <si>
+    <t>Spectral Clustering</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +117,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -113,11 +162,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA9D08E"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA9D08E"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA9D08E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -127,11 +251,109 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -158,66 +380,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Summary graphs.xlsx]Sheet1!PivotTable1</c:name>
-    <c:fmtId val="2"/>
+    <c:name>[Summary graphs.xlsx]Unnormalized!PivotTable1</c:name>
+    <c:fmtId val="15"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="2400" b="1"/>
-              <a:t>Comparison of Clustering Methods for Word Identification</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -385,6 +551,216 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -397,7 +773,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$3:$H$4</c:f>
+              <c:f>Unnormalized!$J$4:$J$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -418,27 +794,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$G$5:$G$12</c:f>
+              <c:f>Unnormalized!$I$6:$I$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Accuracy</c:v>
+                    <c:v>Cophenet</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>Cophenet</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>NMI</c:v>
                   </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Accuracy</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Cophenet</c:v>
-                  </c:pt>
                   <c:pt idx="5">
-                    <c:v>NMI</c:v>
+                    <c:v>Naïve accuracy</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -454,27 +830,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$12</c:f>
+              <c:f>Unnormalized!$J$6:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.19223000000000001</c:v>
+                  <c:v>0.3926</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35527999999999998</c:v>
+                  <c:v>0.51088</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50800999999999996</c:v>
+                  <c:v>0.21262</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13786000000000001</c:v>
+                  <c:v>0.66588000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66588000000000003</c:v>
+                  <c:v>0.37816</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37816</c:v>
+                  <c:v>0.13786000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -485,7 +861,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$4</c:f>
+              <c:f>Unnormalized!$K$4:$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -506,27 +882,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$G$5:$G$12</c:f>
+              <c:f>Unnormalized!$I$6:$I$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Accuracy</c:v>
+                    <c:v>Cophenet</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>Cophenet</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>NMI</c:v>
                   </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Accuracy</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Cophenet</c:v>
-                  </c:pt>
                   <c:pt idx="5">
-                    <c:v>NMI</c:v>
+                    <c:v>Naïve accuracy</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -542,21 +918,185 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$12</c:f>
+              <c:f>Unnormalized!$K$6:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.17379</c:v>
+                <c:pt idx="1">
+                  <c:v>0.55301999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40417999999999998</c:v>
+                  <c:v>0.24640999999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.15340000000000001</c:v>
+                <c:pt idx="4">
+                  <c:v>0.47343000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4672</c:v>
+                  <c:v>0.15437000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Unnormalized!$L$4:$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fuzzy C-Med2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Unnormalized!$I$6:$I$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Cophenet</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cophenet</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>39 MFCCs</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>13 MFCCs</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Unnormalized!$L$6:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.55013999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25806000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48963000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15437000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Unnormalized!$M$4:$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Spectral Clustering</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Unnormalized!$I$6:$I$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Cophenet</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cophenet</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>NMI</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Naïve accuracy</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>39 MFCCs</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>13 MFCCs</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Unnormalized!$M$6:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42770000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13184000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -572,11 +1112,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="281588608"/>
-        <c:axId val="281589784"/>
+        <c:axId val="149557336"/>
+        <c:axId val="149556552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="281588608"/>
+        <c:axId val="149557336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +1144,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -619,7 +1159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281589784"/>
+        <c:crossAx val="149556552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +1167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281589784"/>
+        <c:axId val="149556552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +1203,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -678,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281588608"/>
+        <c:crossAx val="149557336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -706,7 +1246,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -746,7 +1286,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1312,7 +1852,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1323,7 +1863,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654143" cy="6286500"/>
+    <xdr:ext cx="8675077" cy="6301154"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1347,11 +1887,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Fernando Torre" refreshedDate="42346.036364120373" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="22">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Fernando Torre" refreshedDate="42352.98520787037" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="32">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="5">
+  <cacheFields count="7">
     <cacheField name="Dataset" numFmtId="0">
       <sharedItems count="4">
         <s v="39 MFCCs"/>
@@ -1367,22 +1907,31 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Method" numFmtId="0">
-      <sharedItems count="3">
+      <sharedItems count="5">
         <s v="Hierarchical"/>
         <s v="K-Mediods"/>
-        <s v="Fuzzy K-med"/>
+        <s v="Fuzzy C-Med"/>
+        <s v="Spectral Clustering"/>
+        <s v="Fuzzy K-med" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Measure" numFmtId="0">
-      <sharedItems count="4">
+      <sharedItems count="5">
         <s v="NMI"/>
-        <s v="Accuracy"/>
+        <s v="Naïve accuracy"/>
         <s v="Cophenet"/>
+        <s v="Accuracy" u="1"/>
         <s v="Mutual information" u="1"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Value" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.9400000000000001E-3" maxValue="0.8"/>
+    <cacheField name="Unnormalized" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="1.9400000000000001E-3" maxValue="0.8"/>
+    </cacheField>
+    <cacheField name="Normalized" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.13184000000000001" maxValue="0.66588000000000003"/>
+    </cacheField>
+    <cacheField name="% improvement" numFmtId="10">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="-1" maxValue="4.3370786516853927"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1394,13 +1943,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="22">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="32">
   <r>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <n v="6.0699999999999999E-3"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1408,6 +1959,8 @@
     <x v="0"/>
     <x v="1"/>
     <n v="0.50680000000000003"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1415,6 +1968,8 @@
     <x v="0"/>
     <x v="2"/>
     <n v="0.66588000000000003"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1422,6 +1977,8 @@
     <x v="1"/>
     <x v="0"/>
     <n v="1.9400000000000001E-3"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1429,34 +1986,53 @@
     <x v="1"/>
     <x v="1"/>
     <n v="0.52329999999999999"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
-    <n v="0.5"/>
+    <x v="0"/>
+    <s v="too low!"/>
+    <m/>
+    <e v="#VALUE!"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0.39701999999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
-    <n v="0.8"/>
+    <x v="0"/>
+    <n v="0.39701999999999998"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
+    <x v="1"/>
+    <n v="0.8"/>
+    <m/>
+    <n v="-1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="2"/>
     <n v="0.35527999999999998"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
@@ -1464,6 +2040,8 @@
     <x v="1"/>
     <x v="0"/>
     <n v="1.099E-2"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
@@ -1471,34 +2049,53 @@
     <x v="1"/>
     <x v="1"/>
     <n v="0.54271999999999998"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
-    <n v="0.5"/>
+    <x v="0"/>
+    <s v="too low!"/>
+    <m/>
+    <e v="#VALUE!"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0.37816"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <m/>
+    <n v="-1"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <n v="0.13786000000000001"/>
+    <x v="0"/>
+    <n v="0.37816"/>
+    <n v="0.37816"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
+    <x v="1"/>
+    <n v="0.13786000000000001"/>
+    <n v="0.13786000000000001"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <x v="2"/>
     <n v="0.66588000000000003"/>
+    <n v="0.66588000000000003"/>
+    <n v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -1506,6 +2103,8 @@
     <x v="1"/>
     <x v="0"/>
     <n v="0.4672"/>
+    <n v="0.47343000000000002"/>
+    <n v="1.3334760273972623E-2"/>
   </r>
   <r>
     <x v="1"/>
@@ -1513,6 +2112,8 @@
     <x v="1"/>
     <x v="1"/>
     <n v="0.15340000000000001"/>
+    <n v="0.15437000000000001"/>
+    <n v="6.323337679269958E-3"/>
   </r>
   <r>
     <x v="0"/>
@@ -1520,6 +2121,8 @@
     <x v="0"/>
     <x v="0"/>
     <n v="0.50800999999999996"/>
+    <n v="0.51088"/>
+    <n v="5.6494950886794015E-3"/>
   </r>
   <r>
     <x v="0"/>
@@ -1527,6 +2130,8 @@
     <x v="0"/>
     <x v="1"/>
     <n v="0.19223000000000001"/>
+    <n v="0.21262"/>
+    <n v="0.10607085262446025"/>
   </r>
   <r>
     <x v="0"/>
@@ -1534,6 +2139,8 @@
     <x v="0"/>
     <x v="2"/>
     <n v="0.35527999999999998"/>
+    <n v="0.3926"/>
+    <n v="0.10504390902949789"/>
   </r>
   <r>
     <x v="0"/>
@@ -1541,6 +2148,8 @@
     <x v="1"/>
     <x v="0"/>
     <n v="0.40417999999999998"/>
+    <n v="0.55301999999999996"/>
+    <n v="0.36825176901380563"/>
   </r>
   <r>
     <x v="0"/>
@@ -1548,15 +2157,89 @@
     <x v="1"/>
     <x v="1"/>
     <n v="0.17379"/>
+    <n v="0.24640999999999999"/>
+    <n v="0.41786063640025306"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="0.19883000000000001"/>
+    <n v="0.61"/>
+    <n v="2.0679474928330732"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="5.3400000000000003E-2"/>
+    <n v="0.28499999999999998"/>
+    <n v="4.3370786516853927"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="0.41637000000000002"/>
+    <n v="0.42770000000000002"/>
+    <n v="2.7211374498643082E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0.12620999999999999"/>
+    <n v="0.13184000000000001"/>
+    <n v="4.4608192694715276E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0.48963000000000001"/>
+    <n v="0.48963000000000001"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.15437000000000001"/>
+    <n v="0.15437000000000001"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0.38849"/>
+    <n v="0.55013999999999996"/>
+    <n v="0.41609822646657557"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.16408"/>
+    <n v="0.25806000000000001"/>
+    <n v="0.57276938078985862"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="G3:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="22">
+  <location ref="I4:M13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <items count="4">
         <item m="1" x="2"/>
         <item m="1" x="3"/>
@@ -1571,21 +2254,26 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
+      <items count="5">
+        <item n="Fuzzy C-Med" m="1" x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item n="Fuzzy C-Med2" x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="5">
+        <item m="1" x="3"/>
         <item x="2"/>
+        <item m="1" x="4"/>
         <item x="0"/>
         <item x="1"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item m="1" x="3"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="0"/>
@@ -1596,7 +2284,16 @@
       <x v="2"/>
     </i>
     <i r="1">
-      <x/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i r="1">
       <x v="1"/>
@@ -1604,50 +2301,117 @@
     <i r="1">
       <x v="3"/>
     </i>
-    <i>
-      <x v="3"/>
-    </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
+      <x v="4"/>
     </i>
   </rowItems>
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="4">
     <i>
       <x v="1"/>
     </i>
     <i>
       <x v="2"/>
     </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="1" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of Value" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Normalized" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="7">
-    <chartFormat chart="2" format="8" series="1">
+  <formats count="3">
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="17">
+    <chartFormat chart="15" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="9" series="1">
+    <chartFormat chart="15" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="21" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1659,7 +2423,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="10" series="1">
+    <chartFormat chart="15" format="22" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1671,7 +2435,31 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="10" format="11" series="1">
+    <chartFormat chart="15" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="25" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1683,7 +2471,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="10" format="12" series="1">
+    <chartFormat chart="20" format="26" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1695,7 +2483,31 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="11" format="13" series="1">
+    <chartFormat chart="20" format="27" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="28" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="21" format="29" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1707,7 +2519,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="11" format="14" series="1">
+    <chartFormat chart="21" format="30" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1715,6 +2527,30 @@
           </reference>
           <reference field="2" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="21" format="31" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="21" format="32" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -1730,14 +2566,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Dataset"/>
-    <tableColumn id="2" name="Clustering"/>
-    <tableColumn id="3" name="Method"/>
-    <tableColumn id="4" name="Measure"/>
-    <tableColumn id="5" name="Value"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="A1:G33"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Dataset" dataDxfId="15"/>
+    <tableColumn id="2" name="Clustering" dataDxfId="14"/>
+    <tableColumn id="3" name="Method" dataDxfId="13"/>
+    <tableColumn id="4" name="Measure" dataDxfId="12"/>
+    <tableColumn id="5" name="Unnormalized" dataDxfId="11"/>
+    <tableColumn id="6" name="Normalized" dataDxfId="10"/>
+    <tableColumn id="7" name="% improvement" dataDxfId="9">
+      <calculatedColumnFormula>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1786,7 +2626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1821,7 +2661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2006,506 +2846,1002 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" activeCellId="1" sqref="E2 E19"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="16" width="13.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5">
+        <v>6.0699999999999999E-3</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.66588000000000003</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1.9400000000000001E-3</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.52329999999999999</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="12" t="e">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.3926</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.51088</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.55301999999999996</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.55013999999999996</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.39701999999999998</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.21262</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.24640999999999999</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.25806000000000001</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.35527999999999998</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.66588000000000003</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1.099E-2</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.37816</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.47343000000000002</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.48963000000000001</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.42770000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.54271999999999998</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.13786000000000001</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.15437000000000001</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.15437000000000001</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.13184000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="12" t="e">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>-1</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.37816</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.37816</v>
+      </c>
+      <c r="G16" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.13786000000000001</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.13786000000000001</v>
+      </c>
+      <c r="G17" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="J17">
+        <f>J7/J11-1</f>
+        <v>-0.4104042770469154</v>
+      </c>
+      <c r="K17" t="e">
+        <f>K7/K11-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" t="e">
+        <f>L7/L11-1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.66588000000000003</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.66588000000000003</v>
+      </c>
+      <c r="G18" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="J18">
+        <f t="shared" ref="J18" si="0">J8/J12-1</f>
+        <v>0.35096255553204991</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:L20" si="1">K8/K12-1</f>
+        <v>0.168113554274127</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0.1235831137797927</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
-        <v>6.0699999999999999E-3</v>
+      <c r="D19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.4672</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.47343000000000002</v>
+      </c>
+      <c r="G19" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>1.3334760273972623E-2</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="J19">
+        <f t="shared" ref="J19" si="2">J9/J13-1</f>
+        <v>0.54228927897867396</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>0.59622983740364055</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>0.67169786875688287</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>0.50680000000000003</v>
-      </c>
-      <c r="G3" s="1" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.15340000000000001</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.15437000000000001</v>
+      </c>
+      <c r="G20" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>6.323337679269958E-3</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="J20" t="e">
+        <f t="shared" ref="J20" si="3">J10/J14-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.50800999999999996</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.51088</v>
+      </c>
+      <c r="G21" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>5.6494950886794015E-3</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.19223000000000001</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.21262</v>
+      </c>
+      <c r="G22" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.10607085262446025</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="E23" s="5">
+        <v>0.35527999999999998</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.3926</v>
+      </c>
+      <c r="G23" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.10504390902949789</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.40417999999999998</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.55301999999999996</v>
+      </c>
+      <c r="G24" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.36825176901380563</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="E25" s="5">
+        <v>0.17379</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.24640999999999999</v>
+      </c>
+      <c r="G25" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.41786063640025306</v>
+      </c>
+      <c r="H25" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>0.66588000000000003</v>
-      </c>
-      <c r="G4" s="1" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="E26" s="14">
+        <v>0.19883000000000001</v>
+      </c>
+      <c r="F26" s="15">
+        <v>0.61</v>
+      </c>
+      <c r="G26" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>2.0679474928330732</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="B27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="14">
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="F27" s="15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G27" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>4.3370786516853927</v>
+      </c>
+      <c r="H27" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0.41637000000000002</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.42770000000000002</v>
+      </c>
+      <c r="G28" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>2.7211374498643082E-2</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.12620999999999999</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.13184000000000001</v>
+      </c>
+      <c r="G29" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>4.4608192694715276E-2</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0.48963000000000001</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0.48963000000000001</v>
+      </c>
+      <c r="G30" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="14">
+        <v>0.15437000000000001</v>
+      </c>
+      <c r="F31" s="17">
+        <v>0.15437000000000001</v>
+      </c>
+      <c r="G31" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>1.9400000000000001E-3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="14">
+        <v>0.38849</v>
+      </c>
+      <c r="F32" s="15">
+        <v>0.55013999999999996</v>
+      </c>
+      <c r="G32" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.41609822646657557</v>
+      </c>
+      <c r="H32" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>0.52329999999999999</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.19223000000000001</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0.17379</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.35527999999999998</v>
-      </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>0.39701999999999998</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.50800999999999996</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0.40417999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>0.8</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>0.35527999999999998</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.13786000000000001</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0.15340000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>1.099E-2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.66588000000000003</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>0.54271999999999998</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.37816</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0.4672</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14">
-        <v>0.37816</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>0.13786000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>0.66588000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17">
-        <v>0.4672</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>0.15340000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19">
-        <v>0.50800999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>0.19223000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>0.35527999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22">
-        <v>0.40417999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <v>0.17379</v>
-      </c>
+      <c r="B33" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="15">
+        <v>0.16408</v>
+      </c>
+      <c r="F33" s="15">
+        <v>0.25806000000000001</v>
+      </c>
+      <c r="G33" s="12">
+        <f>Table1[[#This Row],[Normalized]]/Table1[[#This Row],[Unnormalized]]-1</f>
+        <v>0.57276938078985862</v>
+      </c>
+      <c r="H33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>